<commit_message>
aggiustati valori 0 per nuovi fondi
</commit_message>
<xml_diff>
--- a/dati_podio.xlsx
+++ b/dati_podio.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dionisie.Turcanu\Documents\GitHub\Dashboard_ER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancamediolanum-my.sharepoint.com/personal/william_marzo_mediolanum_it/Documents/Desktop/Progetti GitHub/Dashboard_ER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D26D471-C39B-4642-8089-FCDFCA9B67EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{5D26D471-C39B-4642-8089-FCDFCA9B67EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48CC6F5F-A3A2-459D-AE80-BCF4610B310E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="x dashboard" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'x dashboard'!$A$1:$CE$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'x dashboard'!$A$1:$CE$72</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1111,15 +1111,16 @@
   <dimension ref="A1:CE72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.7265625" customWidth="1"/>
+    <col min="1" max="1" width="63.77734375" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>91.571428571428569</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>85.142857142857139</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>83.142857142857139</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>80.857142857142861</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>78.285714285714306</v>
       </c>
     </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>75.714285714285722</v>
       </c>
     </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>74.714285714285708</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -3378,7 +3379,7 @@
         <v>73.428571428571445</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>73.428571428571431</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -3880,7 +3881,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -4131,7 +4132,7 @@
         <v>69.857142857142861</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>69.714285714285722</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -4440,12 +4441,66 @@
       <c r="S14">
         <v>4.1996082596782447E-3</v>
       </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
       <c r="Z14">
         <v>-2.5109554068827311E-3</v>
       </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
       <c r="AG14">
         <v>2.514129799259401E-2</v>
       </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
       <c r="AN14">
         <v>0.81660684522163618</v>
       </c>
@@ -4579,7 +4634,7 @@
         <v>67.857142857142861</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -4794,7 +4849,7 @@
         <v>66.714285714285722</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>132</v>
       </c>
@@ -5036,7 +5091,7 @@
         <v>62.285714285714292</v>
       </c>
     </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5287,7 +5342,7 @@
         <v>62.285714285714278</v>
       </c>
     </row>
-    <row r="18" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -5538,7 +5593,7 @@
         <v>62.142857142857153</v>
       </c>
     </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -5789,7 +5844,7 @@
         <v>61.714285714285722</v>
       </c>
     </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -5847,12 +5902,66 @@
       <c r="S20">
         <v>-1.1713014895116339E-2</v>
       </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
       <c r="Z20">
         <v>-7.2484777977235293E-3</v>
       </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
       <c r="AG20">
         <v>1.8784084023429681E-2</v>
       </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
       <c r="AN20">
         <v>-1.2587604641054071</v>
       </c>
@@ -5986,7 +6095,7 @@
         <v>61.714285714285722</v>
       </c>
     </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -6237,7 +6346,7 @@
         <v>61.285714285714292</v>
       </c>
     </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -6461,7 +6570,7 @@
         <v>60.428571428571431</v>
       </c>
     </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -6519,12 +6628,66 @@
       <c r="S23">
         <v>-2.305356748597398E-2</v>
       </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
       <c r="Z23">
         <v>-3.800960116839835E-3</v>
       </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
       <c r="AG23">
         <v>7.0671378091873294E-3</v>
       </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
       <c r="AN23">
         <v>-2.7378259762977541</v>
       </c>
@@ -6658,7 +6821,7 @@
         <v>60.285714285714292</v>
       </c>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -6909,7 +7072,7 @@
         <v>60.534535345350001</v>
       </c>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -7160,7 +7323,7 @@
         <v>59.142857142857153</v>
       </c>
     </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -7411,7 +7574,7 @@
         <v>58.857142857142847</v>
       </c>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -7662,7 +7825,7 @@
         <v>58.285714285714292</v>
       </c>
     </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -7913,7 +8076,7 @@
         <v>56.285714285714292</v>
       </c>
     </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -8164,7 +8327,7 @@
         <v>56.142857142857139</v>
       </c>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -8415,7 +8578,7 @@
         <v>54.571428571428569</v>
       </c>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -8666,7 +8829,7 @@
         <v>54.285714285714278</v>
       </c>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -8917,7 +9080,7 @@
         <v>52.571428571428569</v>
       </c>
     </row>
-    <row r="33" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -9168,7 +9331,7 @@
         <v>52.428571428571431</v>
       </c>
     </row>
-    <row r="34" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -9419,7 +9582,7 @@
         <v>50.714285714285722</v>
       </c>
     </row>
-    <row r="35" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -9670,7 +9833,7 @@
         <v>49.571428571428569</v>
       </c>
     </row>
-    <row r="36" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>136</v>
       </c>
@@ -9921,7 +10084,7 @@
         <v>49.571428571428569</v>
       </c>
     </row>
-    <row r="37" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -10172,7 +10335,7 @@
         <v>48.571428571428569</v>
       </c>
     </row>
-    <row r="38" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -10423,7 +10586,7 @@
         <v>47.428571428571431</v>
       </c>
     </row>
-    <row r="39" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>139</v>
       </c>
@@ -10674,7 +10837,7 @@
         <v>46.857142857142847</v>
       </c>
     </row>
-    <row r="40" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -10925,7 +11088,7 @@
         <v>46.714285714285722</v>
       </c>
     </row>
-    <row r="41" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -11176,7 +11339,7 @@
         <v>46.571428571428569</v>
       </c>
     </row>
-    <row r="42" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -11427,7 +11590,7 @@
         <v>46.142857142857139</v>
       </c>
     </row>
-    <row r="43" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>133</v>
       </c>
@@ -11678,7 +11841,7 @@
         <v>45.428571428571431</v>
       </c>
     </row>
-    <row r="44" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>114</v>
       </c>
@@ -11929,7 +12092,7 @@
         <v>45.285714285714278</v>
       </c>
     </row>
-    <row r="45" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -12180,7 +12343,7 @@
         <v>45.142857142857153</v>
       </c>
     </row>
-    <row r="46" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>113</v>
       </c>
@@ -12431,7 +12594,7 @@
         <v>44.428571428571423</v>
       </c>
     </row>
-    <row r="47" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -12682,7 +12845,7 @@
         <v>43.285714285714292</v>
       </c>
     </row>
-    <row r="48" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -12933,7 +13096,7 @@
         <v>42.857142857142847</v>
       </c>
     </row>
-    <row r="49" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -13184,7 +13347,7 @@
         <v>42.285714285714278</v>
       </c>
     </row>
-    <row r="50" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -13435,7 +13598,7 @@
         <v>41.571428571428569</v>
       </c>
     </row>
-    <row r="51" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -13686,7 +13849,7 @@
         <v>41.142857142857139</v>
       </c>
     </row>
-    <row r="52" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>148</v>
       </c>
@@ -13901,7 +14064,7 @@
         <v>39.428571428571438</v>
       </c>
     </row>
-    <row r="53" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -14152,7 +14315,7 @@
         <v>39.285714285714292</v>
       </c>
     </row>
-    <row r="54" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -14403,7 +14566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -14654,7 +14817,7 @@
         <v>35.571428571428569</v>
       </c>
     </row>
-    <row r="56" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -14905,7 +15068,7 @@
         <v>35.285714285714278</v>
       </c>
     </row>
-    <row r="57" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -15156,7 +15319,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -15407,7 +15570,7 @@
         <v>34.428571428571431</v>
       </c>
     </row>
-    <row r="59" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -15658,7 +15821,7 @@
         <v>31.857142857142861</v>
       </c>
     </row>
-    <row r="60" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -15909,7 +16072,7 @@
         <v>31.571428571428569</v>
       </c>
     </row>
-    <row r="61" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -16160,7 +16323,7 @@
         <v>30.571428571428569</v>
       </c>
     </row>
-    <row r="62" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -16411,7 +16574,7 @@
         <v>29.857142857142851</v>
       </c>
     </row>
-    <row r="63" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -16662,7 +16825,7 @@
         <v>29.714285714285719</v>
       </c>
     </row>
-    <row r="64" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -16913,7 +17076,7 @@
         <v>28.571428571428569</v>
       </c>
     </row>
-    <row r="65" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>98</v>
       </c>
@@ -17164,7 +17327,7 @@
         <v>28.142857142857139</v>
       </c>
     </row>
-    <row r="66" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>110</v>
       </c>
@@ -17415,7 +17578,7 @@
         <v>26.142857142857139</v>
       </c>
     </row>
-    <row r="67" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -17666,7 +17829,7 @@
         <v>23.285714285714281</v>
       </c>
     </row>
-    <row r="68" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -17908,7 +18071,7 @@
         <v>19.571428571428569</v>
       </c>
     </row>
-    <row r="69" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -18159,7 +18322,7 @@
         <v>19.142857142857149</v>
       </c>
     </row>
-    <row r="70" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>126</v>
       </c>
@@ -18410,7 +18573,7 @@
         <v>19.142857142857139</v>
       </c>
     </row>
-    <row r="71" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -18661,7 +18824,7 @@
         <v>15.857142857142859</v>
       </c>
     </row>
-    <row r="72" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -18913,7 +19076,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CE1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:CE72" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CE72">
       <sortCondition descending="1" ref="CE1"/>
     </sortState>

</xml_diff>